<commit_message>
#6 updates template for ecoinvent 3.8
</commit_message>
<xml_diff>
--- a/import_template.xlsx
+++ b/import_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rhanes\GitHub\autoBW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{144FA2DC-8797-4325-B4C6-907A5D3E21E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E337F1BA-D23B-4B8C-B3DC-B32E51BC18AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28965" yWindow="3150" windowWidth="15945" windowHeight="12045" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28830" yWindow="1065" windowWidth="16020" windowHeight="11715" tabRatio="527" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Create Activities" sheetId="5" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Add Exchanges" sheetId="4" r:id="rId3"/>
     <sheet name="Delete Exchanges" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="52">
   <si>
     <t>US</t>
   </si>
@@ -42,57 +42,30 @@
     <t>kg</t>
   </si>
   <si>
-    <t>ecoinvent 3.7.1 consequential</t>
-  </si>
-  <si>
     <t>lubricating oil production</t>
   </si>
   <si>
-    <t>1e9857fe7e9c88bbbaff87b7fd322d4e</t>
-  </si>
-  <si>
     <t>market group for diesel</t>
   </si>
   <si>
     <t>market for steel, chromium steel 18/8</t>
   </si>
   <si>
-    <t>186e19fa6465514ebe6243b36382520a</t>
-  </si>
-  <si>
     <t>transport, freight train</t>
   </si>
   <si>
-    <t>1f54ef3533e0ca95122c1f869428c541</t>
-  </si>
-  <si>
     <t>cement production, Portland</t>
   </si>
   <si>
-    <t>ffd6836cd82ac339b36616cbb9dd6ff4</t>
-  </si>
-  <si>
     <t>market for gypsum, mineral</t>
   </si>
   <si>
-    <t>0733b2583ae87bebc1bb4a64798ade38</t>
-  </si>
-  <si>
     <t>market for electricity, medium voltage</t>
   </si>
   <si>
     <t>electric grid mix</t>
   </si>
   <si>
-    <t>04b818d7946b8689c96aaea50d6a076f</t>
-  </si>
-  <si>
-    <t>market for transmission network, electricity, medium voltage</t>
-  </si>
-  <si>
-    <t>43251df807f82a95b6c475078e4ba12c</t>
-  </si>
-  <si>
     <t>2-Methyl pentane, from chemistry, at plant</t>
   </si>
   <si>
@@ -141,9 +114,6 @@
     <t>code</t>
   </si>
   <si>
-    <t>ecoinvent3.7.1 cut-off</t>
-  </si>
-  <si>
     <t>borax production, anhydrous, powder</t>
   </si>
   <si>
@@ -153,9 +123,6 @@
     <t>RoW</t>
   </si>
   <si>
-    <t>c7bcb2c135dd16e83fd249ad4dc1d966</t>
-  </si>
-  <si>
     <t>activity</t>
   </si>
   <si>
@@ -181,6 +148,48 @@
   </si>
   <si>
     <t>source_database</t>
+  </si>
+  <si>
+    <t>ecoinvent3.8</t>
+  </si>
+  <si>
+    <t>52fac57961930c641d849a8e01e54ca0</t>
+  </si>
+  <si>
+    <t>64b1bbdb0e404fa074271fb09e844b3e</t>
+  </si>
+  <si>
+    <t>791d43943f97d7490f7bc8d498a8d309</t>
+  </si>
+  <si>
+    <t>580b7aea44c188e5958b4c6bd6ec515a</t>
+  </si>
+  <si>
+    <t>95eda656d8f8fbf6c2740b583df64778</t>
+  </si>
+  <si>
+    <t>28868487d550b40cec2a4163343345b5</t>
+  </si>
+  <si>
+    <t>eba30d382c566eb39aa7436807938e4e</t>
+  </si>
+  <si>
+    <t>8f93cae3c51d4c58246e14044feab023</t>
+  </si>
+  <si>
+    <t>a35e530f0b0dda90f5f64da0a0b3e901</t>
+  </si>
+  <si>
+    <t>transmission network, electricity, medium voltage</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>destination_database</t>
+  </si>
+  <si>
+    <t>activity_type</t>
   </si>
 </sst>
 </file>
@@ -664,11 +673,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1024,114 +1032,130 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{277CB9D4-0D4C-4491-B6C5-72355C9F8902}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
         <v>20</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
         <v>21</v>
       </c>
-      <c r="E1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
         <v>23</v>
       </c>
-      <c r="G1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
         <v>19</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>2</v>
-      </c>
-      <c r="G2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" t="s">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" t="s">
-        <v>0</v>
-      </c>
-      <c r="H4">
+      <c r="H4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4">
         <v>0.1</v>
       </c>
     </row>
@@ -1142,11 +1166,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C672BCA2-5B17-4648-9C3C-2F437DABBC60}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1155,30 +1177,78 @@
     <col min="3" max="3" width="34.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
         <v>39</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1186,7 +1256,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB2043D1-6EE9-43E0-B324-EF1E0EADF96E}">
   <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -1206,37 +1276,37 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>41</v>
+      <c r="J1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" t="s">
+        <v>30</v>
       </c>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -1245,13 +1315,13 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G2">
         <v>0.8</v>
@@ -1263,64 +1333,64 @@
         <v>0</v>
       </c>
       <c r="J2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="G3">
         <v>0.1</v>
       </c>
       <c r="H3" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="I3" t="s">
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="G4">
         <v>4</v>
       </c>
       <c r="H4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="I4" t="s">
         <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="E5" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="G5">
         <v>0.2</v>
@@ -1332,18 +1402,18 @@
         <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G6">
         <v>0.01</v>
@@ -1355,33 +1425,33 @@
         <v>0</v>
       </c>
       <c r="J6" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="E7" t="s">
         <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="G7">
         <v>0.5</v>
       </c>
       <c r="H7" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="I7" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="J7" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="K7" t="s">
         <v>39</v>
@@ -1389,36 +1459,36 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="E8" t="s">
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="G8">
         <v>3</v>
       </c>
       <c r="H8" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="I8" t="s">
         <v>0</v>
       </c>
       <c r="J8" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="E9" t="s">
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G9">
         <v>0.78</v>
@@ -1430,7 +1500,7 @@
         <v>0</v>
       </c>
       <c r="J9" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1444,7 +1514,7 @@
   <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1458,25 +1528,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G1" s="1"/>
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>49</v>
+      </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -1489,83 +1561,71 @@
       <c r="Q1" s="1"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="F2" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="F3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D5" t="s">
-        <v>2</v>
+        <v>38</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates database name to refer to ecoinvent 3.8 cut-off
</commit_message>
<xml_diff>
--- a/import_template.xlsx
+++ b/import_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rhanes\GitHub\autoBW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E337F1BA-D23B-4B8C-B3DC-B32E51BC18AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A534B454-CDB1-4B07-9E7C-DE8C7196E9F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28830" yWindow="1065" windowWidth="16020" windowHeight="11715" tabRatio="527" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="950" yWindow="0" windowWidth="18250" windowHeight="10800" tabRatio="527" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Create Activities" sheetId="5" r:id="rId1"/>
@@ -150,9 +150,6 @@
     <t>source_database</t>
   </si>
   <si>
-    <t>ecoinvent3.8</t>
-  </si>
-  <si>
     <t>52fac57961930c641d849a8e01e54ca0</t>
   </si>
   <si>
@@ -190,6 +187,9 @@
   </si>
   <si>
     <t>activity_type</t>
+  </si>
+  <si>
+    <t>ecoinvent 3.8 cut-off</t>
   </si>
 </sst>
 </file>
@@ -1038,26 +1038,26 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" customWidth="1"/>
-    <col min="3" max="3" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.54296875" customWidth="1"/>
+    <col min="3" max="3" width="39.7265625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.54296875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C1" t="s">
         <v>29</v>
@@ -1084,10 +1084,10 @@
         <v>25</v>
       </c>
       <c r="K1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>36</v>
       </c>
@@ -1113,7 +1113,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>36</v>
       </c>
@@ -1136,7 +1136,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>36</v>
       </c>
@@ -1168,16 +1168,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C672BCA2-5B17-4648-9C3C-2F437DABBC60}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>37</v>
       </c>
@@ -1188,62 +1190,62 @@
         <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
         <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1256,25 +1258,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB2043D1-6EE9-43E0-B324-EF1E0EADF96E}">
   <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="40" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="34.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>31</v>
       </c>
@@ -1313,7 +1315,7 @@
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="C2" t="s">
         <v>9</v>
       </c>
@@ -1336,7 +1338,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="C3" t="s">
         <v>9</v>
       </c>
@@ -1359,7 +1361,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="C4" t="s">
         <v>20</v>
       </c>
@@ -1382,7 +1384,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="C5" t="s">
         <v>20</v>
       </c>
@@ -1405,7 +1407,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="C6" t="s">
         <v>20</v>
       </c>
@@ -1428,9 +1430,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="C7" t="s">
         <v>20</v>
@@ -1454,10 +1456,10 @@
         <v>36</v>
       </c>
       <c r="K7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="C8" t="s">
         <v>22</v>
       </c>
@@ -1480,7 +1482,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="C9" t="s">
         <v>22</v>
       </c>
@@ -1513,21 +1515,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0948324-ADD0-429A-AD05-3510BCB3C5ED}">
   <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="56.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="56.7265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="34" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>31</v>
       </c>
@@ -1547,7 +1549,7 @@
         <v>30</v>
       </c>
       <c r="G1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -1560,72 +1562,72 @@
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="E2" t="s">
         <v>3</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="E3" t="s">
         <v>5</v>
       </c>
       <c r="F3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>8</v>
       </c>
       <c r="C5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" t="s">
         <v>46</v>
-      </c>
-      <c r="D5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F5" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>